<commit_message>
measurement units, new script init
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkv465\Documents\GitHub\NHANES_T2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\GitHub\NHANES_T2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3636"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Framingham Offspring</t>
-  </si>
-  <si>
-    <t>Fasting plasma glucose level, BMI, high density lipoprotein cholesterol level, parental history of diabetes, triglyceride level, blood pressure</t>
   </si>
   <si>
     <t>USA</t>
@@ -370,18 +367,6 @@
     <t>Aekplakorn et. al. (EGATS)</t>
   </si>
   <si>
-    <t>South India</t>
-  </si>
-  <si>
-    <t>https://www.researchgate.net/publication/7434301_A_simplified_Indian_Diabetes_Risk_Score_for_screening_for_undiagnosed_diabetic_subjects</t>
-  </si>
-  <si>
-    <t>Physical Activity included in the risk model, Vasquez does not mention it, see the link ----&gt;</t>
-  </si>
-  <si>
-    <t>Mohan et. al.</t>
-  </si>
-  <si>
     <t>Mauritians Indians</t>
   </si>
   <si>
@@ -440,6 +425,21 @@
   </si>
   <si>
     <t>Table 2 in https://www.liebertpub.com/doi/epub/10.1089/dia.2010.0106</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fasting plasma glucose level, BMI, high density lipoprotein cholesterol level, parental history of diabetes, triglyceride level, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>systolic and diastolic blood pressure, antihypertensive treatment</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -490,16 +490,14 @@
       <family val="1"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,12 +524,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -657,11 +649,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -709,40 +700,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -771,8 +751,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1051,345 +1030,325 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="16" customWidth="1"/>
     <col min="3" max="3" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.33203125" style="16" customWidth="1"/>
-    <col min="6" max="8" width="20.88671875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="16"/>
+    <col min="4" max="5" width="12.36328125" style="16" customWidth="1"/>
+    <col min="6" max="8" width="20.90625" style="16" customWidth="1"/>
+    <col min="9" max="16384" width="8.90625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>7</v>
+      <c r="H1" s="25" t="s">
+        <v>6</v>
       </c>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
     </row>
-    <row r="2" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+    <row r="2" spans="1:11" ht="145" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>14</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:11" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="20" t="s">
+    <row r="3" spans="1:11" ht="82.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="20" t="s">
+      <c r="H3" s="17" t="s">
         <v>19</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>20</v>
       </c>
       <c r="J3" s="15"/>
       <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="D4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="F4" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="H4" s="17" t="s">
         <v>42</v>
-      </c>
-      <c r="G4" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>43</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
-    <row r="5" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B5" s="20" t="s">
+    <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="20" t="s">
+      <c r="H5" s="17" t="s">
         <v>30</v>
-      </c>
-      <c r="H5" s="20" t="s">
-        <v>31</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="C6" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="20" t="s">
+      <c r="F6" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>37</v>
+      <c r="G6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="20" t="s">
+    <row r="7" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="20" t="s">
+      <c r="F7" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>45</v>
       </c>
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="22">
+        <v>2011</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="26">
+      <c r="D8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="22">
+        <v>2009</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="22">
+        <v>2008</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" s="22">
         <v>2011</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="18">
-        <v>2005</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="C11" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G11" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="26">
-        <v>2009</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="22" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="26">
-        <v>2008</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="H11" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="26">
-        <v>2011</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="H12" s="22" t="s">
-        <v>107</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I9" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1401,205 +1360,205 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="34" t="s">
+      <c r="B2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="30"/>
+      <c r="B3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="30"/>
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="30"/>
+      <c r="B5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="6" t="s">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="30"/>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="31"/>
+      <c r="B7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
-      <c r="B6" s="4" t="s">
+      <c r="B10" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="33"/>
+      <c r="B11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="33"/>
+      <c r="B12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="33"/>
+      <c r="B13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="33"/>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="33"/>
+      <c r="B15" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="36"/>
-      <c r="B7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="6" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="33"/>
+      <c r="B16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="34"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="39"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="10" t="s">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="11" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="93" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="11" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
table update, removal of findrisk
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="97">
   <si>
     <t>Framingham Offspring</t>
   </si>
@@ -91,21 +91,6 @@
     <t>5-year risk</t>
   </si>
   <si>
-    <t>Lindström et. al, 2013 (FINDRISC)</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>Finland</t>
-  </si>
-  <si>
-    <t>67%</t>
-  </si>
-  <si>
-    <t>13-year risk</t>
-  </si>
-  <si>
     <t>Balkau et. al. (DESIR Score)</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
   </si>
   <si>
     <t>85% Non-Hispanic Whites</t>
-  </si>
-  <si>
-    <t>Table 1 in https://doi.org/10.2337/diacare.26.3.725</t>
   </si>
   <si>
     <t>7.5-year risk</t>
@@ -438,15 +420,12 @@
       <t>systolic and diastolic blood pressure, antihypertensive treatment</t>
     </r>
   </si>
-  <si>
-    <t>Age, BMI, Waist circumference, Use of antihypertensive treatment, history of high blood glycose</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,13 +450,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF131413"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -652,7 +624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -707,9 +679,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,28 +1016,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="24" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="15"/>
@@ -1091,7 +1060,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>12</v>
@@ -1104,7 +1073,7 @@
     </row>
     <row r="3" spans="1:11" ht="82.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>17</v>
@@ -1116,10 +1085,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>18</v>
@@ -1131,8 +1100,8 @@
       <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="20" t="s">
-        <v>21</v>
+      <c r="A4" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>22</v>
@@ -1144,51 +1113,51 @@
         <v>16</v>
       </c>
       <c r="E4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>25</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>41</v>
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15"/>
     </row>
-    <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
-        <v>81</v>
+    <row r="5" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C5" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>97</v>
-      </c>
       <c r="F5" s="17" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="21" t="s">
-        <v>31</v>
+    <row r="6" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>32</v>
@@ -1197,153 +1166,125 @@
         <v>1</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>33</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="B7" s="21">
+        <v>2011</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>85</v>
+        <v>40</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="22">
+        <v>84</v>
+      </c>
+      <c r="B8" s="21">
+        <v>2009</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="21">
+        <v>2008</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="21">
         <v>2011</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="22">
-        <v>2009</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="24" t="s">
+      <c r="C10" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="19" t="s">
+      <c r="E10" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" s="22">
-        <v>2008</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="19" t="s">
+      <c r="F10" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>20</v>
-      </c>
       <c r="H10" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="22">
-        <v>2011</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="24" t="s">
         <v>95</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1371,194 +1312,194 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="29"/>
+      <c r="B3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="29"/>
+      <c r="B4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="29"/>
+      <c r="B5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="29"/>
+      <c r="B6" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="30"/>
+      <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="30"/>
-      <c r="B3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A4" s="30"/>
-      <c r="B4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="30"/>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="30"/>
-      <c r="B6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31"/>
-      <c r="B7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="32"/>
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="32"/>
+      <c r="B12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="32"/>
+      <c r="B13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="32"/>
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="32"/>
+      <c r="B15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="32"/>
+      <c r="B16" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="33"/>
-      <c r="B11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
-      <c r="A13" s="33"/>
-      <c r="B13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="33"/>
-      <c r="B14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="33"/>
-      <c r="B15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="33"/>
-      <c r="B16" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="34"/>
+      <c r="A17" s="33"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+        <v>69</v>
+      </c>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+        <v>70</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
diabetes definition change, excel update
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>Framingham Offspring</t>
   </si>
@@ -85,9 +85,6 @@
     <t>9-year risk</t>
   </si>
   <si>
-    <t>5-year risk</t>
-  </si>
-  <si>
     <t>Balkau et. al. (DESIR Score)</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>12-year risk</t>
   </si>
   <si>
-    <t>Statistical Analysis section and Table 3 in https://doi.org/10.2337/dc05-2141</t>
-  </si>
-  <si>
     <t>Schmidt et. al. (ARIC Score)</t>
   </si>
   <si>
@@ -112,12 +106,6 @@
     <t xml:space="preserve">56% </t>
   </si>
   <si>
-    <t>Age, Waist circumference, height, systolic blood pressure, Family history of diabetes, Ethnicity, Fasting plasma glucose level, HDL, Triglycerides</t>
-  </si>
-  <si>
-    <t>Age, BMI,  Waist circumference,  Hypertension,  Family history of diabetes in first degree relative</t>
-  </si>
-  <si>
     <t>Table 1 in https://doi.org/10.2337/diacare.28.8.2013</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t>7.5-year risk</t>
   </si>
   <si>
-    <t>Table 2 in https://doi.org/10.7326/0003-4819-136-8-200204160-00006</t>
-  </si>
-  <si>
     <t>Rosella et. Al. (DPoRT)</t>
   </si>
   <si>
@@ -152,12 +137,6 @@
   </si>
   <si>
     <t>53.6%</t>
-  </si>
-  <si>
-    <t>Age, Ethnicity, BMI, Hypertension, Immigrant status, Smoking, Education, Cardiovascular disease</t>
-  </si>
-  <si>
-    <t>Figure 1 in doi:10.1136/jech.2009.102244</t>
   </si>
   <si>
     <t>Study</t>
@@ -349,36 +328,9 @@
     <t>53.42%</t>
   </si>
   <si>
-    <t>Age, Gender, Ethnicity, Fasting plasma glucose level, Systolic blood pressure, High density lipoprotein cholesterol level, BMI, Family history of diabetes in first degree relative</t>
-  </si>
-  <si>
-    <t>Table 2 in https://onlinelibrary.wiley.com/doi/epdf/10.1111/j.1464-5491.2009.02810.x</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>54.77%</t>
-  </si>
-  <si>
-    <t>100% Non Hispanic Whites</t>
-  </si>
-  <si>
     <t>Gao et. al. (NS Score)</t>
   </si>
   <si>
-    <t>Cameron et. al. (AusDiab)</t>
-  </si>
-  <si>
-    <t>BMI, Waist circumference, Family history of diabetes</t>
-  </si>
-  <si>
-    <t>Age, Gender, Ethnicity, Fasting plasma glucose level, Systolic blood pressure, High density lipoprotein cholesterol level, BMI, Parental history of diabetes</t>
-  </si>
-  <si>
-    <t>Table 3 in https://onlinelibrary.wiley.com/doi/epdf/10.1111/j.1365-2796.2008.01935.x</t>
-  </si>
-  <si>
     <t>10-year risk</t>
   </si>
   <si>
@@ -394,9 +346,6 @@
     <t>China</t>
   </si>
   <si>
-    <t>Age, Hypertension, History of high blood glucose level, BMI, Fasting plasma glucose level, Triglyceride level, High density lipoprotein cholesterol level</t>
-  </si>
-  <si>
     <t>Table 2 in https://www.liebertpub.com/doi/epub/10.1089/dia.2010.0106</t>
   </si>
   <si>
@@ -413,16 +362,6 @@
   </si>
   <si>
     <t>Ready?</t>
-  </si>
-  <si>
-    <t>- Sex
-- Fasting glucose
-- BMI
-- HDL-C
-- Parental history of diabetes
-- Triglycerides
-- Systolic and diastolic blood pressure
-- Antihypertensive treatment</t>
   </si>
   <si>
     <t>- Sex
@@ -433,6 +372,87 @@
   </si>
   <si>
     <t>Table 3 in https://doi.org/10.2337/dc08-0368</t>
+  </si>
+  <si>
+    <t>- Sex
+- Age
+- BMI
+- Waist circumference
+- Hypertension
+- Family history of diabetes (parents/sibling)</t>
+  </si>
+  <si>
+    <t>Table 3 in https://doi.org/10.2337/dc05-2141</t>
+  </si>
+  <si>
+    <t>- Sex
+- Fasting glucose
+- BMI
+- HDL-C
+- Family history of diabetes (parent)
+- Triglycerides
+- Systolic and diastolic blood pressure
+- Antihypertensive treatment</t>
+  </si>
+  <si>
+    <t>- Age
+- Race
+- Family history of diabetes (parent)
+- Fasting glucose
+- Systolic blood pressure
+- Waist circumference
+- Height
+- HDL-C
+- Triglycerides</t>
+  </si>
+  <si>
+    <t>Appendix in https://doi.org/10.7326/0003-4819-136-8-200204160-00006</t>
+  </si>
+  <si>
+    <t>- Sex
+- Age
+- Ethnicity
+- Fasting glucose
+- Systolic blood pressure
+- HDL-C
+- BMI
+- Family history of diabetes (parent/sibling)</t>
+  </si>
+  <si>
+    <t>- Sex
+- Age
+- Ethnicity
+- BMI
+- Hypertension
+- Immigrant status
+- Smoking status
+- Education
+- Cardiovascular disease</t>
+  </si>
+  <si>
+    <t>Table 2 (men), Table 3 (women), and Figure 1 in doi:10.1136/jech.2009.102244</t>
+  </si>
+  <si>
+    <t>- Sex
+- Age
+- BMI
+- Waist circumference
+- Family history of diabetes</t>
+  </si>
+  <si>
+    <t>Figure 1 in https://onlinelibrary.wiley.com/doi/epdf/10.1111/j.1464-5491.2009.02810.x</t>
+  </si>
+  <si>
+    <t>is this model named?</t>
+  </si>
+  <si>
+    <t>- Age
+- Hypertension
+- History of high blood glucose level
+- BMI
+Fasting  glucose
+- Triglycerides
+- HDL-C</t>
   </si>
 </sst>
 </file>
@@ -462,13 +482,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
@@ -476,14 +489,22 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +535,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -686,59 +713,55 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1031,306 +1054,281 @@
     <col min="2" max="2" width="12" style="16" customWidth="1"/>
     <col min="3" max="3" width="16" style="16" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.36328125" style="16" customWidth="1"/>
-    <col min="6" max="8" width="20.90625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="20.90625" style="31" customWidth="1"/>
+    <col min="7" max="8" width="20.90625" style="16" customWidth="1"/>
     <col min="9" max="16384" width="8.90625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" ht="24.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="26" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="32" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="120.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="32" t="s">
+      <c r="F2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="30" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:12" ht="60.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:12" ht="84.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="15"/>
+    </row>
+    <row r="5" spans="1:12" ht="120.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:12" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="32">
+        <v>2011</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="60.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="32">
+        <v>2009</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A3" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="32" t="s">
+    </row>
+    <row r="9" spans="1:12" ht="96.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="32">
+        <v>2011</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="K3" s="15"/>
-    </row>
-    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="E9" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="K4" s="15"/>
-    </row>
-    <row r="5" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" ht="116" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="29">
-        <v>2011</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="29">
-        <v>2009</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="31" t="s">
+      <c r="G9" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="29">
-        <v>2008</v>
-      </c>
-      <c r="C9" s="31" t="s">
+      <c r="J9" s="15" t="s">
         <v>79</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="101.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="29">
-        <v>2011</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>87</v>
-      </c>
-      <c r="H10" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1358,194 +1356,194 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="21"/>
+      <c r="B3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+      <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="21"/>
+      <c r="B5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="22"/>
+      <c r="B7" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="22"/>
-      <c r="B3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
-      <c r="B5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="22"/>
-      <c r="B6" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="23"/>
-      <c r="B7" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="8"/>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="24"/>
+      <c r="B11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="24"/>
+      <c r="B12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="9" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="24"/>
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
-      <c r="B11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="6" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
+        <v>57</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
       <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
       <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+        <v>58</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
       <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="26"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
+        <v>61</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+        <v>62</v>
+      </c>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alex Framingham double checked
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -325,9 +325,6 @@
     <t>Alex</t>
   </si>
   <si>
-    <t>Tibor</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -440,9 +437,6 @@
     <t>EGATS Risk Score (Aekplakorn et al.)</t>
   </si>
   <si>
-    <t>ARIC Model (Schmidt et al.)</t>
-  </si>
-  <si>
     <t>San Antonio Model (Stern et al.)</t>
   </si>
   <si>
@@ -453,13 +447,42 @@
   </si>
   <si>
     <t>Chinese Diabetes Risk Score (Liu et al.)</t>
+  </si>
+  <si>
+    <t>Thea</t>
+  </si>
+  <si>
+    <r>
+      <t>ARIC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Model - Clinical variables plus fasting glucose and lipids </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Schmidt et al.)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,6 +524,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1037,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1078,15 +1108,15 @@
         <v>5</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>4</v>
@@ -1101,7 +1131,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>11</v>
@@ -1116,7 +1146,7 @@
     </row>
     <row r="3" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>16</v>
@@ -1131,13 +1161,13 @@
         <v>31</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J3" s="15" t="s">
         <v>68</v>
@@ -1146,7 +1176,7 @@
     </row>
     <row r="4" spans="1:11" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>18</v>
@@ -1161,22 +1191,22 @@
         <v>64</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>21</v>
@@ -1191,7 +1221,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>17</v>
@@ -1200,13 +1230,13 @@
         <v>23</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>24</v>
@@ -1221,22 +1251,22 @@
         <v>25</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B7" s="23">
         <v>2011</v>
@@ -1251,50 +1281,50 @@
         <v>32</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B8" s="23">
         <v>2009</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="25" t="s">
         <v>62</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8" s="25" t="s">
         <v>61</v>
       </c>
       <c r="H8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="96.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B9" s="23">
         <v>2011</v>
@@ -1309,7 +1339,7 @@
         <v>65</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G9" s="25" t="s">
         <v>63</v>
@@ -1318,7 +1348,7 @@
         <v>67</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DPoRT and Gao scores
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfr661\Documents\GitHub\NHANES_T2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfp688\Documents\GitHub\NHANES_T2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <t>USA</t>
   </si>
@@ -301,9 +301,6 @@
     </r>
   </si>
   <si>
-    <t>11-year risk</t>
-  </si>
-  <si>
     <t>53.42%</t>
   </si>
   <si>
@@ -476,6 +473,15 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Questions sent to corresponding author</t>
+  </si>
+  <si>
+    <t>Out: no reported intercept and one of the predictors is "history of high blood glucose", i.e. diabetes or latent diabetes - which makes no sense...</t>
+  </si>
+  <si>
+    <t>Instantaneous risk (hazard)</t>
   </si>
 </sst>
 </file>
@@ -689,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -758,6 +764,9 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -803,9 +812,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -843,7 +852,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -915,7 +924,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1067,22 +1076,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="16" customWidth="1"/>
     <col min="3" max="3" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.42578125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="22" customWidth="1"/>
-    <col min="7" max="8" width="20.85546875" style="16" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="16"/>
+    <col min="4" max="5" width="12.453125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="22" customWidth="1"/>
+    <col min="7" max="8" width="20.81640625" style="16" customWidth="1"/>
+    <col min="9" max="10" width="8.81640625" style="16"/>
+    <col min="11" max="11" width="11.26953125" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -1108,15 +1119,15 @@
         <v>5</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="K1" s="15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="132.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>4</v>
@@ -1131,7 +1142,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" s="18" t="s">
         <v>11</v>
@@ -1140,13 +1151,13 @@
         <v>12</v>
       </c>
       <c r="J2" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K2" s="15"/>
     </row>
-    <row r="3" spans="1:11" ht="72.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>16</v>
@@ -1161,22 +1172,22 @@
         <v>31</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>18</v>
@@ -1188,27 +1199,27 @@
         <v>15</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J4" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="120.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>21</v>
@@ -1223,7 +1234,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="18" t="s">
         <v>17</v>
@@ -1232,13 +1243,13 @@
         <v>23</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="120.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>24</v>
@@ -1253,22 +1264,22 @@
         <v>25</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G6" s="18" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="108.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="23">
         <v>2011</v>
@@ -1283,74 +1294,80 @@
         <v>32</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="72.75" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A8" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="23">
         <v>2009</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>81</v>
-      </c>
       <c r="J8" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="96.75" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="96.5" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="23">
         <v>2011</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="25" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G9" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>83</v>
+      <c r="K9" s="16" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1367,16 +1384,16 @@
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1393,177 +1410,177 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="30" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="27" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="31"/>
       <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="31"/>
       <c r="B4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="31"/>
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="31"/>
       <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="32"/>
       <c r="B7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="33" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="27" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="34"/>
       <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="34"/>
       <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="34"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="34"/>
       <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="34"/>
       <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="33"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="34"/>
       <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="34"/>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="35"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="11" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
Cross-checked Lex + cleaning
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkv465\Documents\GitHub\NHANES_T2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cfp688\Documents\GitHub\NHANES_T2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>USA</t>
   </si>
@@ -483,6 +483,9 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>Out: specifically developped for Mauritian Indians (explicitly mentionned); also, absolute probabilities not calculable from Cox since outcome is not all-cause mortality</t>
+  </si>
 </sst>
 </file>
 
@@ -540,7 +543,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +574,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -695,7 +704,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -763,7 +772,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -794,6 +802,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1076,24 +1099,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="16" customWidth="1"/>
     <col min="3" max="3" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.77734375" style="16" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" style="16"/>
-    <col min="11" max="11" width="11.21875" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.77734375" style="16"/>
+    <col min="4" max="5" width="12.453125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.81640625" style="16" customWidth="1"/>
+    <col min="9" max="10" width="8.81640625" style="16"/>
+    <col min="11" max="11" width="11.1796875" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1148,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>85</v>
       </c>
@@ -1157,7 +1180,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>86</v>
       </c>
@@ -1189,7 +1212,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="84.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>87</v>
       </c>
@@ -1221,7 +1244,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="120.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>93</v>
       </c>
@@ -1251,7 +1274,7 @@
       </c>
       <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="108.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>88</v>
       </c>
@@ -1281,7 +1304,7 @@
       </c>
       <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:11" ht="108.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A7" s="18" t="s">
         <v>90</v>
       </c>
@@ -1309,68 +1332,71 @@
       <c r="J7" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="60.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:11" s="39" customFormat="1" ht="60.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="36">
         <v>2009</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="H8" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="40" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="K8" s="41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="39" customFormat="1" ht="96.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="36">
         <v>2011</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="39" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1388,16 +1414,16 @@
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1414,177 +1440,177 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="30"/>
       <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="31"/>
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
+      <c r="A4" s="30"/>
       <c r="B4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
       <c r="E4" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="31"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="30"/>
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="30"/>
       <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="32"/>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="31"/>
       <c r="B7" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="32" t="s">
         <v>48</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="34"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="33"/>
       <c r="B11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="34"/>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="33"/>
       <c r="B12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="34"/>
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
+      <c r="A13" s="33"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="34"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="33"/>
       <c r="B14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="34"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="33"/>
       <c r="B15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="34"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="33"/>
       <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="35"/>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="34"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
       <c r="E20" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
       <c r="E22" s="11" t="s">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
model check, removing DPORT
</commit_message>
<xml_diff>
--- a/Table_T2D_predmodels.xlsx
+++ b/Table_T2D_predmodels.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkv465\Documents\GitHub\NHANES_T2D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\GitHub\NHANES_T2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="3650"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ms table" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="moved or excluded models" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="100">
   <si>
     <t>USA</t>
   </si>
@@ -1100,26 +1101,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.54296875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="16" customWidth="1"/>
     <col min="3" max="3" width="16" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.44140625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="20.77734375" style="16" customWidth="1"/>
-    <col min="9" max="10" width="8.77734375" style="16"/>
-    <col min="11" max="11" width="11.21875" style="16" customWidth="1"/>
-    <col min="12" max="16384" width="8.77734375" style="16"/>
+    <col min="4" max="5" width="12.453125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="20.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.81640625" style="16" customWidth="1"/>
+    <col min="9" max="10" width="8.81640625" style="16"/>
+    <col min="11" max="11" width="11.1796875" style="16" customWidth="1"/>
+    <col min="12" max="16384" width="8.81640625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="24.5" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="132.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>85</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="60.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="60.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>86</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="84.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="84.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>87</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="120.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="120.5" x14ac:dyDescent="0.35">
       <c r="A5" s="21" t="s">
         <v>93</v>
       </c>
@@ -1275,9 +1276,11 @@
       <c r="J5" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="K5" s="15"/>
-    </row>
-    <row r="6" spans="1:11" ht="108.6" x14ac:dyDescent="0.3">
+      <c r="K5" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>88</v>
       </c>
@@ -1305,102 +1308,8 @@
       <c r="J6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="K6" s="15"/>
-    </row>
-    <row r="7" spans="1:11" ht="108.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B7" s="23">
-        <v>2011</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="30" customFormat="1" ht="60.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="27">
-        <v>2009</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>80</v>
-      </c>
-      <c r="J8" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="30" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="27">
-        <v>2011</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="K9" s="30" t="s">
-        <v>95</v>
+      <c r="K6" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1417,16 +1326,16 @@
       <selection activeCell="C2" sqref="C2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1443,7 +1352,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1369,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="37"/>
       <c r="B3" s="4" t="s">
         <v>40</v>
@@ -1469,7 +1378,7 @@
       <c r="D3" s="34"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="52" x14ac:dyDescent="0.35">
       <c r="A4" s="37"/>
       <c r="B4" s="4" t="s">
         <v>41</v>
@@ -1480,7 +1389,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="37"/>
       <c r="B5" s="4" t="s">
         <v>42</v>
@@ -1489,7 +1398,7 @@
       <c r="D5" s="34"/>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="37"/>
       <c r="B6" s="4" t="s">
         <v>43</v>
@@ -1498,7 +1407,7 @@
       <c r="D6" s="34"/>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="38"/>
       <c r="B7" s="5" t="s">
         <v>44</v>
@@ -1507,8 +1416,8 @@
       <c r="D7" s="35"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="39" t="s">
         <v>48</v>
       </c>
@@ -1523,7 +1432,7 @@
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="40"/>
       <c r="B11" s="4" t="s">
         <v>50</v>
@@ -1532,7 +1441,7 @@
       <c r="D11" s="34"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="40"/>
       <c r="B12" s="4" t="s">
         <v>51</v>
@@ -1543,7 +1452,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="78" x14ac:dyDescent="0.35">
       <c r="A13" s="40"/>
       <c r="B13" s="4" t="s">
         <v>52</v>
@@ -1554,7 +1463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="40"/>
       <c r="B14" s="4" t="s">
         <v>53</v>
@@ -1563,7 +1472,7 @@
       <c r="D14" s="34"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="40"/>
       <c r="B15" s="4" t="s">
         <v>44</v>
@@ -1572,7 +1481,7 @@
       <c r="D15" s="34"/>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="40"/>
       <c r="B16" s="4" t="s">
         <v>54</v>
@@ -1581,15 +1490,15 @@
       <c r="D16" s="34"/>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="41"/>
       <c r="B17" s="5"/>
       <c r="C17" s="35"/>
       <c r="D17" s="35"/>
       <c r="E17" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>57</v>
       </c>
@@ -1600,14 +1509,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="13"/>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:5" ht="93" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="91.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="14" t="s">
         <v>58</v>
       </c>
@@ -1632,4 +1541,115 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B6:B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:11" s="16" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="23">
+        <v>2011</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="30" customFormat="1" ht="60.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="27">
+        <v>2009</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="30" customFormat="1" ht="96.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="27">
+        <v>2011</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>